<commit_message>
data update, removed keyboard
</commit_message>
<xml_diff>
--- a/t_set_test.xlsx
+++ b/t_set_test.xlsx
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:X101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>